<commit_message>
Open registration for NextGen Event & recompile
</commit_message>
<xml_diff>
--- a/data/roster_nextgen.xlsx
+++ b/data/roster_nextgen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10608"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/widmelu1/Documents/git/bbs-basel/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD462D79-5B8D-AA4A-9AC8-85E696BF8ED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A19E33F-3386-8948-9974-31D04AB77E40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="48240" yWindow="-520" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2020 Roster" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
   <si>
     <t>Company</t>
   </si>
@@ -36,9 +36,6 @@
     <t>F. Hoffmann-La Roche Ltd</t>
   </si>
   <si>
-    <t>Swiss Tropical and Public Health Institute</t>
-  </si>
-  <si>
     <t>Novartis Pharma AG</t>
   </si>
   <si>
@@ -121,6 +118,15 @@
   </si>
   <si>
     <t>Former</t>
+  </si>
+  <si>
+    <t>Nikki</t>
+  </si>
+  <si>
+    <t>Rommers</t>
+  </si>
+  <si>
+    <t>University Hospital of Basel</t>
   </si>
 </sst>
 </file>
@@ -495,7 +501,7 @@
   <dimension ref="A1:T21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="101.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -513,36 +519,36 @@
   <sheetData>
     <row r="1" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="G1" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="C2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E2" s="2">
         <v>1</v>
@@ -551,13 +557,13 @@
     </row>
     <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="2">
@@ -567,10 +573,10 @@
     </row>
     <row r="4" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>1</v>
@@ -582,13 +588,13 @@
     </row>
     <row r="5" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="C5" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E5" s="2">
         <v>1</v>
@@ -597,10 +603,10 @@
     </row>
     <row r="6" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>1</v>
@@ -612,13 +618,13 @@
     </row>
     <row r="7" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="C7" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E7" s="2">
         <v>1</v>
@@ -627,11 +633,11 @@
     </row>
     <row r="8" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="C8" s="1" t="s">
         <v>1</v>
       </c>
@@ -639,18 +645,18 @@
         <v>1</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="C9" s="1" t="s">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="E9" s="2">
         <v>1</v>
@@ -659,20 +665,32 @@
     </row>
     <row r="10" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="C10" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E10" s="2">
         <v>1</v>
       </c>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="2">
+        <v>1</v>
+      </c>
       <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>